<commit_message>
Cucumber POM,BDD framework finished
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
   <si>
     <t>Login with valid username and password</t>
   </si>
@@ -27,6 +27,18 @@
   </si>
   <si>
     <t>Create Country</t>
+  </si>
+  <si>
+    <t>States testing with JDBC</t>
+  </si>
+  <si>
+    <t>21.09.22</t>
+  </si>
+  <si>
+    <t>22.09.22</t>
+  </si>
+  <si>
+    <t>FAILED</t>
   </si>
 </sst>
 </file>
@@ -71,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -105,6 +117,132 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Jenkins Default test çalıştırılması için, RunnerClass a plugin ve POM xml eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="10">
   <si>
     <t>Login with valid username and password</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>FAILED</t>
+  </si>
+  <si>
+    <t>12.10.22</t>
   </si>
 </sst>
 </file>
@@ -83,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -243,6 +246,34 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>